<commit_message>
feat: support loading from specific XLSX worksheets
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/oligos.xlsx
+++ b/tests/mock_excel_db/oligos.xlsx
@@ -8,14 +8,14 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Oligos" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Trash" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ignore" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Oligos" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Oligos!$I$94:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Oligos"</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Sheet_Title" vbProcedure="false">"Trash"</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Oligos!$I$94:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Trash"</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Sheet_Title" vbProcedure="false">"Oligos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Tag</t>
   </si>
@@ -75,48 +75,6 @@
   </si>
   <si>
     <t xml:space="preserve">HPLC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41_TM62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tttatacagttcatccatgccatc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove repA from 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverse PCR: product=43 template=27 primers=41,42 Ta=62 len=2974 tx=2min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42_TM61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tgaaagtgatctcctcagaataatc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove repA and mWasabi from 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverse PCR: product=45 template=27 primers=42,43 Ta=62 len=2269 tx=1m30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43_TM62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggcgcctttttcgaac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove mWasabi from 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverse PCR: product=44 template=27 primers=43,44 Ta=63 len=3121 tx=2min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44_TM62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actgatcttcaccaaacgtattac</t>
   </si>
 </sst>
 </file>
@@ -235,15 +193,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="B1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Sans,Regular"&amp;K000000&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Sans,Regular"&amp;K000000Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.19"/>
@@ -326,97 +321,4 @@
     <oddFooter>&amp;C&amp;"Sans,Regular"&amp;K000000Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.45"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <f aca="false">LEN(B1)</f>
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">LEN(B2)</f>
-        <v>25</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">LEN(B3)</f>
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">LEN(B4)</f>
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Sans,Regular"&amp;K000000&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Sans,Regular"&amp;K000000Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>